<commit_message>
Update languages comparsion sheet
</commit_message>
<xml_diff>
--- a/Comparsion.xlsx
+++ b/Comparsion.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
   <si>
     <t>Сравнение языков</t>
   </si>
@@ -113,13 +113,92 @@
   <si>
     <t>10k звезд git-hub
 npm-совместим</t>
+  </si>
+  <si>
+    <t>Типизация</t>
+  </si>
+  <si>
+    <t>Опыт написания кода, цикл обратной связи, достаточность инструментов</t>
+  </si>
+  <si>
+    <t>Иммутабельность</t>
+  </si>
+  <si>
+    <t>Сигнатуры исчезают после компиляции, система стипов допускает погрешности, иногда требует ручного указания</t>
+  </si>
+  <si>
+    <t>+ -</t>
+  </si>
+  <si>
+    <t>Кротчайшая обратная связь: рекомпиляция - затянуто но терпимо. Достаточный stdlib, широкая поддержка IDE</t>
+  </si>
+  <si>
+    <t>Только при const и readonly</t>
+  </si>
+  <si>
+    <t>Простейшее решение: guard и :pre b :post секции - довольно удобно, можно определять спецификации любой сложности. Не хватает подсказки по типам в IDE. Для подробных спецификаций есть spec, но код на нем страшный как чума.</t>
+  </si>
+  <si>
+    <t>Код пишется быстро, быстрая ОС через REPL, но требуется reload файла. Достаточный и приятный stdlib, широкаяя поддержка IDE.</t>
+  </si>
+  <si>
+    <t>Все иммутабельно по умолчанию</t>
+  </si>
+  <si>
+    <t>Недостаточно инструментов для писания в иммутабельном стиле.</t>
+  </si>
+  <si>
+    <t>Долгая настройка, ручная настройка каждого target-файла. Рекомпиляцию по одному target-файлу за раз.</t>
+  </si>
+  <si>
+    <t>Строгая типизация, богатая система типов. Автовывод типов, поэтому код не перегружен.</t>
+  </si>
+  <si>
+    <t>Быстрая рекомпиляция с проверкой типов. Достаточная коллекция библиотек. Поддержка IDE, Конвейеры облегчают написание кода.</t>
+  </si>
+  <si>
+    <t>Понятен и приятен, благодаря избыточности библиотек, удачной конвенции неймингов и конвейерам</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Σ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
+  </si>
+  <si>
+    <t>Σ 5,5</t>
+  </si>
+  <si>
+    <t>Σ 4,5</t>
+  </si>
+  <si>
+    <t>Σ 7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +221,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -179,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -188,9 +275,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -199,6 +283,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,199 +582,303 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="5" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" customWidth="1"/>
-    <col min="9" max="9" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" customWidth="1"/>
+    <col min="7" max="7" width="6" style="9" customWidth="1"/>
+    <col min="8" max="8" width="32.5703125" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" style="9" customWidth="1"/>
+    <col min="10" max="10" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="I4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>29</v>
       </c>
     </row>
+    <row r="8" spans="1:10" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>